<commit_message>
Upload same file with changes
Updated cell B2 to Yes
</commit_message>
<xml_diff>
--- a/Excel Github Test1.xlsx
+++ b/Excel Github Test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CJ\The Data Scientist's Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D67E297-E697-4B9C-946C-018F9302726A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5D5F93-7EDA-4437-A93E-45AFA70B1324}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{AC34496C-F573-40DE-B3DE-A51E924C9682}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>test 1</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
 </sst>
 </file>
@@ -396,7 +393,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +411,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>